<commit_message>
Ausarbeitung: Boxplots und Tabelle beschrieben sowie die Tabelle noch ein wenig angepasst.
</commit_message>
<xml_diff>
--- a/Dokumente/Neue_Messungen/Messungen_als_Tabelle.xlsx
+++ b/Dokumente/Neue_Messungen/Messungen_als_Tabelle.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bauer\Desktop\bvrc_rbn\Dokumente\Neue_Messungen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7308F871-061C-4FBA-88A4-AEEF79A1E708}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15238366-D826-4482-A1EE-6AEEE00FD5DA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{FD2D6849-4FEF-4336-9892-3E4AA58E6B72}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Bonsai</t>
   </si>
@@ -59,19 +59,25 @@
     <t>DDC. m. v. S.a.r.</t>
   </si>
   <si>
-    <t>Messdauer in s</t>
-  </si>
-  <si>
-    <t>Ø Kernel in ms</t>
-  </si>
-  <si>
-    <t>Ø Overhead in ms</t>
+    <t>Varianz</t>
+  </si>
+  <si>
+    <t>Ø K. in ms</t>
+  </si>
+  <si>
+    <t>Ø Oh. in ms</t>
+  </si>
+  <si>
+    <t>Md. in s</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -89,7 +95,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -237,7 +243,7 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -253,22 +259,22 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -317,19 +323,6 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -340,7 +333,6 @@
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -350,26 +342,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -684,275 +677,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{533B4BF9-4ABF-4C7B-AC99-74FBCA746AAD}">
-  <dimension ref="A9:J17"/>
+  <dimension ref="A9:M17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="210" zoomScaleNormal="210" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="16.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="16.42578125" customWidth="1"/>
-    <col min="10" max="10" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="7.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" customWidth="1"/>
+    <col min="7" max="7" width="6.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="11" max="11" width="6.85546875" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="12"/>
-      <c r="B10" s="2" t="s">
+    <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="2" t="s">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="3"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="2" t="s">
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="4"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="2"/>
+      <c r="M10" s="3"/>
     </row>
-    <row r="11" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="17"/>
-      <c r="B11" s="18" t="s">
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="E11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="H11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="19" t="s">
+      <c r="K11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="L11" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="I11" s="19" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="20" t="s">
-        <v>9</v>
+      <c r="M11" s="10" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B12" s="14">
+      <c r="B12" s="12">
         <v>36.9297857876712</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="13">
+        <v>2.7355242671877902E-3</v>
+      </c>
+      <c r="D12" s="13">
         <v>9.8253511986301305</v>
       </c>
-      <c r="D12" s="16">
+      <c r="E12" s="14">
         <v>27.305</v>
       </c>
-      <c r="E12" s="14">
+      <c r="F12" s="12">
         <v>82.126394691780803</v>
       </c>
-      <c r="F12" s="15">
+      <c r="G12" s="13">
+        <v>2.1701532766173199E-3</v>
+      </c>
+      <c r="H12" s="13">
         <v>10.954084760273901</v>
       </c>
-      <c r="G12" s="16">
+      <c r="I12" s="14">
         <v>54.359000000000002</v>
       </c>
-      <c r="H12" s="14">
+      <c r="J12" s="12">
         <v>77.709999999999994</v>
       </c>
-      <c r="I12" s="15">
+      <c r="K12" s="13">
+        <v>4.6107147016208397E-2</v>
+      </c>
+      <c r="L12" s="13">
         <v>10.089339383561599</v>
       </c>
-      <c r="J12" s="16">
+      <c r="M12" s="14">
         <v>51.276000000000003</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="15">
         <v>29.848280993150599</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="16">
+        <v>2.6366526077722998</v>
+      </c>
+      <c r="D13" s="16">
         <v>9.6945272260273896</v>
       </c>
-      <c r="D13" s="6">
+      <c r="E13" s="17">
         <v>23.093</v>
       </c>
-      <c r="E13" s="5">
+      <c r="F13" s="15">
         <v>63.457712671232798</v>
       </c>
-      <c r="F13" s="1">
+      <c r="G13" s="16">
+        <v>19.3733780095654</v>
+      </c>
+      <c r="H13" s="16">
         <v>10.7785886986301</v>
       </c>
-      <c r="G13" s="6">
+      <c r="I13" s="17">
         <v>43.353999999999999</v>
       </c>
-      <c r="H13" s="5">
+      <c r="J13" s="15">
         <v>60.34</v>
       </c>
-      <c r="I13" s="1">
+      <c r="K13" s="16">
+        <v>11.2898221295772</v>
+      </c>
+      <c r="L13" s="16">
         <v>10.3660306506849</v>
       </c>
-      <c r="J13" s="6">
+      <c r="M13" s="17">
         <v>41.290999999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="15">
         <v>14.2043962328767</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="16">
+        <v>4.2407049079994996</v>
+      </c>
+      <c r="D14" s="16">
         <v>12.2493708904109</v>
       </c>
-      <c r="D14" s="6">
+      <c r="E14" s="17">
         <v>15.449</v>
       </c>
-      <c r="E14" s="5">
+      <c r="F14" s="15">
         <v>30.741174657534199</v>
       </c>
-      <c r="F14" s="1">
+      <c r="G14" s="16">
+        <v>13.1711600059673</v>
+      </c>
+      <c r="H14" s="16">
         <v>13.2451267123287</v>
       </c>
-      <c r="G14" s="6">
+      <c r="I14" s="17">
         <v>25.687999999999999</v>
       </c>
-      <c r="H14" s="5">
+      <c r="J14" s="15">
         <v>34.78</v>
       </c>
-      <c r="I14" s="1">
+      <c r="K14" s="16">
+        <v>5.8811498036631802</v>
+      </c>
+      <c r="L14" s="16">
         <v>14.9226467465753</v>
       </c>
-      <c r="J14" s="6">
+      <c r="M14" s="17">
         <v>29.024999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="15">
         <v>11.6994787842465</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="16">
+        <v>5.4735917874846498</v>
+      </c>
+      <c r="D15" s="16">
         <v>11.8878499828767</v>
       </c>
-      <c r="D15" s="6">
+      <c r="E15" s="17">
         <v>13.775</v>
       </c>
-      <c r="E15" s="5">
+      <c r="F15" s="15">
         <v>24.902526198630099</v>
       </c>
-      <c r="F15" s="1">
+      <c r="G15" s="16">
+        <v>21.605288884433399</v>
+      </c>
+      <c r="H15" s="16">
         <v>12.684802568493099</v>
       </c>
-      <c r="G15" s="6">
+      <c r="I15" s="17">
         <v>21.951000000000001</v>
       </c>
-      <c r="H15" s="5">
+      <c r="J15" s="15">
         <v>27.55</v>
       </c>
-      <c r="I15" s="1">
+      <c r="K15" s="16">
+        <v>11.045061473142599</v>
+      </c>
+      <c r="L15" s="16">
         <v>12.5283840753424</v>
       </c>
-      <c r="J15" s="6">
+      <c r="M15" s="17">
         <v>23.408000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="15">
         <v>11.028516575342399</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="16">
+        <v>24.4282335500797</v>
+      </c>
+      <c r="D16" s="16">
         <v>16.707784794520499</v>
       </c>
-      <c r="D16" s="6">
+      <c r="E16" s="17">
         <v>16.198</v>
       </c>
-      <c r="E16" s="5">
+      <c r="F16" s="15">
         <v>23.047051027397199</v>
       </c>
-      <c r="F16" s="1">
+      <c r="G16" s="16">
+        <v>40.3412603655811</v>
+      </c>
+      <c r="H16" s="16">
         <v>19.048839383561599</v>
       </c>
-      <c r="G16" s="6">
+      <c r="I16" s="17">
         <v>24.584</v>
       </c>
-      <c r="H16" s="5">
+      <c r="J16" s="15">
         <v>30.12</v>
       </c>
-      <c r="I16" s="1">
+      <c r="K16" s="16">
+        <v>62.086483999150303</v>
+      </c>
+      <c r="L16" s="16">
         <v>20.295353938356101</v>
       </c>
-      <c r="J16" s="6">
+      <c r="M16" s="17">
         <v>29.45</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+    <row r="17" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="7">
+      <c r="B17" s="18">
         <v>9.8507901541095801</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="19">
+        <v>22.366012925830901</v>
+      </c>
+      <c r="D17" s="19">
         <v>16.279346832191699</v>
       </c>
-      <c r="D17" s="9">
+      <c r="E17" s="20">
         <v>15.26</v>
       </c>
-      <c r="E17" s="7">
+      <c r="F17" s="18">
         <v>20.407421558219099</v>
       </c>
-      <c r="F17" s="8">
+      <c r="G17" s="19">
+        <v>38.809151757070303</v>
+      </c>
+      <c r="H17" s="19">
         <v>18.131962003424601</v>
       </c>
-      <c r="G17" s="9">
+      <c r="I17" s="20">
         <v>22.507000000000001</v>
       </c>
-      <c r="H17" s="7">
+      <c r="J17" s="18">
         <v>26.31</v>
       </c>
-      <c r="I17" s="8">
+      <c r="K17" s="19">
+        <v>58.257150152237202</v>
+      </c>
+      <c r="L17" s="19">
         <v>19.815770547945199</v>
       </c>
-      <c r="J17" s="9">
+      <c r="M17" s="20">
         <v>26.934999999999999</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="E10:G10"/>
-    <mergeCell ref="H10:J10"/>
     <mergeCell ref="A10:A11"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="B10:E10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>